<commit_message>
Agrego datos otorgadas pd 2021. Agrego nota de datos faltantes en figuras
</commit_message>
<xml_diff>
--- a/data/Datos_serie_historica_KS_CONICET.xlsx
+++ b/data/Datos_serie_historica_KS_CONICET.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="31">
   <si>
     <t>Convocatoria</t>
   </si>
@@ -196,6 +196,9 @@
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -207,9 +210,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -4719,7 +4719,9 @@
         <v>10</v>
       </c>
       <c r="E181" s="6"/>
-      <c r="F181" s="6"/>
+      <c r="F181" s="10">
+        <v>14.0</v>
+      </c>
       <c r="G181" s="6"/>
     </row>
     <row r="182">
@@ -4736,7 +4738,9 @@
         <v>10</v>
       </c>
       <c r="E182" s="6"/>
-      <c r="F182" s="6"/>
+      <c r="F182" s="10">
+        <v>24.0</v>
+      </c>
       <c r="G182" s="6"/>
     </row>
     <row r="183">
@@ -4753,7 +4757,9 @@
         <v>10</v>
       </c>
       <c r="E183" s="6"/>
-      <c r="F183" s="6"/>
+      <c r="F183" s="10">
+        <v>16.0</v>
+      </c>
       <c r="G183" s="6"/>
     </row>
     <row r="184">
@@ -4770,7 +4776,9 @@
         <v>10</v>
       </c>
       <c r="E184" s="6"/>
-      <c r="F184" s="6"/>
+      <c r="F184" s="10">
+        <v>23.0</v>
+      </c>
       <c r="G184" s="6"/>
     </row>
     <row r="185">
@@ -4787,7 +4795,9 @@
         <v>10</v>
       </c>
       <c r="E185" s="6"/>
-      <c r="F185" s="6"/>
+      <c r="F185" s="10">
+        <v>36.0</v>
+      </c>
       <c r="G185" s="6"/>
     </row>
     <row r="186">
@@ -4804,7 +4814,9 @@
         <v>10</v>
       </c>
       <c r="E186" s="6"/>
-      <c r="F186" s="6"/>
+      <c r="F186" s="10">
+        <v>6.0</v>
+      </c>
       <c r="G186" s="6"/>
     </row>
     <row r="187">
@@ -4821,7 +4833,9 @@
         <v>10</v>
       </c>
       <c r="E187" s="6"/>
-      <c r="F187" s="6"/>
+      <c r="F187" s="10">
+        <v>16.0</v>
+      </c>
       <c r="G187" s="6"/>
     </row>
     <row r="188">
@@ -4838,7 +4852,9 @@
         <v>10</v>
       </c>
       <c r="E188" s="6"/>
-      <c r="F188" s="6"/>
+      <c r="F188" s="10">
+        <v>10.0</v>
+      </c>
       <c r="G188" s="6"/>
     </row>
     <row r="189">
@@ -4855,7 +4871,9 @@
         <v>10</v>
       </c>
       <c r="E189" s="6"/>
-      <c r="F189" s="6"/>
+      <c r="F189" s="10">
+        <v>15.0</v>
+      </c>
       <c r="G189" s="6"/>
     </row>
     <row r="190">
@@ -4874,6 +4892,9 @@
       <c r="E190" s="6"/>
       <c r="F190" s="6"/>
       <c r="G190" s="6"/>
+      <c r="H190" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="2">
@@ -4889,7 +4910,9 @@
         <v>23</v>
       </c>
       <c r="E191" s="6"/>
-      <c r="F191" s="6"/>
+      <c r="F191" s="10">
+        <v>1.0</v>
+      </c>
       <c r="G191" s="6"/>
     </row>
     <row r="192">
@@ -4923,7 +4946,9 @@
         <v>23</v>
       </c>
       <c r="E193" s="6"/>
-      <c r="F193" s="6"/>
+      <c r="F193" s="10">
+        <v>1.0</v>
+      </c>
       <c r="G193" s="6"/>
     </row>
     <row r="194">
@@ -4940,7 +4965,9 @@
         <v>23</v>
       </c>
       <c r="E194" s="6"/>
-      <c r="F194" s="6"/>
+      <c r="F194" s="10">
+        <v>4.0</v>
+      </c>
       <c r="G194" s="6"/>
     </row>
     <row r="195">
@@ -4957,7 +4984,9 @@
         <v>23</v>
       </c>
       <c r="E195" s="6"/>
-      <c r="F195" s="6"/>
+      <c r="F195" s="10">
+        <v>9.0</v>
+      </c>
       <c r="G195" s="6"/>
     </row>
     <row r="196">
@@ -4974,7 +5003,9 @@
         <v>23</v>
       </c>
       <c r="E196" s="6"/>
-      <c r="F196" s="6"/>
+      <c r="F196" s="10">
+        <v>1.0</v>
+      </c>
       <c r="G196" s="6"/>
     </row>
     <row r="197">
@@ -4991,7 +5022,9 @@
         <v>23</v>
       </c>
       <c r="E197" s="6"/>
-      <c r="F197" s="6"/>
+      <c r="F197" s="10">
+        <v>3.0</v>
+      </c>
       <c r="G197" s="6"/>
     </row>
     <row r="198">
@@ -5008,7 +5041,9 @@
         <v>23</v>
       </c>
       <c r="E198" s="6"/>
-      <c r="F198" s="6"/>
+      <c r="F198" s="10">
+        <v>1.0</v>
+      </c>
       <c r="G198" s="6"/>
     </row>
     <row r="199">
@@ -5025,7 +5060,9 @@
         <v>23</v>
       </c>
       <c r="E199" s="6"/>
-      <c r="F199" s="6"/>
+      <c r="F199" s="10">
+        <v>2.0</v>
+      </c>
       <c r="G199" s="6"/>
     </row>
     <row r="200">
@@ -5044,6 +5081,9 @@
       <c r="E200" s="6"/>
       <c r="F200" s="6"/>
       <c r="G200" s="6"/>
+      <c r="H200" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="2">
@@ -5276,7 +5316,7 @@
       </c>
       <c r="E210" s="4"/>
       <c r="F210" s="4"/>
-      <c r="G210" s="10"/>
+      <c r="G210" s="11"/>
       <c r="H210" s="9" t="s">
         <v>26</v>
       </c>
@@ -5522,7 +5562,7 @@
       </c>
       <c r="E220" s="4"/>
       <c r="F220" s="4"/>
-      <c r="G220" s="10"/>
+      <c r="G220" s="11"/>
       <c r="H220" s="9" t="s">
         <v>26</v>
       </c>
@@ -5757,7 +5797,7 @@
       <c r="D230" s="4"/>
       <c r="E230" s="4"/>
       <c r="F230" s="4"/>
-      <c r="G230" s="10"/>
+      <c r="G230" s="11"/>
       <c r="H230" s="9" t="s">
         <v>26</v>
       </c>
@@ -6012,7 +6052,7 @@
       </c>
       <c r="E240" s="4"/>
       <c r="F240" s="4"/>
-      <c r="G240" s="10"/>
+      <c r="G240" s="11"/>
       <c r="H240" s="9" t="s">
         <v>26</v>
       </c>
@@ -6258,7 +6298,7 @@
       </c>
       <c r="E250" s="4"/>
       <c r="F250" s="4"/>
-      <c r="G250" s="10"/>
+      <c r="G250" s="11"/>
       <c r="H250" s="9" t="s">
         <v>26</v>
       </c>
@@ -6513,7 +6553,7 @@
       </c>
       <c r="E260" s="4"/>
       <c r="F260" s="4"/>
-      <c r="G260" s="10"/>
+      <c r="G260" s="11"/>
       <c r="H260" s="9" t="s">
         <v>26</v>
       </c>
@@ -6768,7 +6808,7 @@
       </c>
       <c r="E270" s="4"/>
       <c r="F270" s="4"/>
-      <c r="G270" s="10"/>
+      <c r="G270" s="11"/>
       <c r="H270" s="9" t="s">
         <v>26</v>
       </c>
@@ -7003,7 +7043,7 @@
       <c r="D280" s="4"/>
       <c r="E280" s="4"/>
       <c r="F280" s="4"/>
-      <c r="G280" s="10"/>
+      <c r="G280" s="11"/>
       <c r="H280" s="9" t="s">
         <v>26</v>
       </c>
@@ -7258,7 +7298,7 @@
       </c>
       <c r="E290" s="4"/>
       <c r="F290" s="4"/>
-      <c r="G290" s="10"/>
+      <c r="G290" s="11"/>
       <c r="H290" s="9" t="s">
         <v>26</v>
       </c>
@@ -7510,7 +7550,7 @@
       </c>
       <c r="E300" s="4"/>
       <c r="F300" s="4"/>
-      <c r="G300" s="10"/>
+      <c r="G300" s="11"/>
       <c r="H300" s="4"/>
       <c r="I300" s="4"/>
       <c r="J300" s="4"/>
@@ -7930,7 +7970,7 @@
       <c r="F321" s="2">
         <v>4.0</v>
       </c>
-      <c r="J321" s="11"/>
+      <c r="J321" s="12"/>
     </row>
     <row r="322">
       <c r="A322" s="2">
@@ -7946,7 +7986,7 @@
       <c r="F322" s="2">
         <v>11.0</v>
       </c>
-      <c r="J322" s="11"/>
+      <c r="J322" s="12"/>
     </row>
     <row r="323">
       <c r="A323" s="2">
@@ -7962,7 +8002,7 @@
       <c r="F323" s="2">
         <v>5.0</v>
       </c>
-      <c r="J323" s="11"/>
+      <c r="J323" s="12"/>
     </row>
     <row r="324">
       <c r="A324" s="2">
@@ -7978,7 +8018,7 @@
       <c r="F324" s="2">
         <v>19.0</v>
       </c>
-      <c r="J324" s="11"/>
+      <c r="J324" s="12"/>
     </row>
     <row r="325">
       <c r="A325" s="2">
@@ -7994,7 +8034,7 @@
       <c r="F325" s="2">
         <v>21.0</v>
       </c>
-      <c r="J325" s="11"/>
+      <c r="J325" s="12"/>
     </row>
     <row r="326">
       <c r="A326" s="2">
@@ -8010,7 +8050,7 @@
       <c r="F326" s="2">
         <v>1.0</v>
       </c>
-      <c r="J326" s="11"/>
+      <c r="J326" s="12"/>
     </row>
     <row r="327">
       <c r="A327" s="2">
@@ -8026,7 +8066,7 @@
       <c r="F327" s="2">
         <v>11.0</v>
       </c>
-      <c r="J327" s="11"/>
+      <c r="J327" s="12"/>
     </row>
     <row r="328">
       <c r="A328" s="2">
@@ -8042,7 +8082,7 @@
       <c r="F328" s="2">
         <v>8.0</v>
       </c>
-      <c r="J328" s="11"/>
+      <c r="J328" s="12"/>
     </row>
     <row r="329">
       <c r="A329" s="2">
@@ -8058,7 +8098,7 @@
       <c r="F329" s="2">
         <v>9.0</v>
       </c>
-      <c r="J329" s="11"/>
+      <c r="J329" s="12"/>
     </row>
     <row r="330">
       <c r="A330" s="9">
@@ -8497,7 +8537,7 @@
       <c r="F351" s="2">
         <v>15.0</v>
       </c>
-      <c r="J351" s="11"/>
+      <c r="J351" s="12"/>
     </row>
     <row r="352">
       <c r="A352" s="2">
@@ -8515,7 +8555,7 @@
       <c r="F352" s="2">
         <v>23.0</v>
       </c>
-      <c r="J352" s="11"/>
+      <c r="J352" s="12"/>
     </row>
     <row r="353">
       <c r="A353" s="2">
@@ -8533,7 +8573,7 @@
       <c r="F353" s="2">
         <v>14.0</v>
       </c>
-      <c r="J353" s="11"/>
+      <c r="J353" s="12"/>
     </row>
     <row r="354">
       <c r="A354" s="2">
@@ -8551,7 +8591,7 @@
       <c r="F354" s="2">
         <v>29.0</v>
       </c>
-      <c r="J354" s="11"/>
+      <c r="J354" s="12"/>
     </row>
     <row r="355">
       <c r="A355" s="2">
@@ -8569,7 +8609,7 @@
       <c r="F355" s="2">
         <v>34.0</v>
       </c>
-      <c r="J355" s="11"/>
+      <c r="J355" s="12"/>
     </row>
     <row r="356">
       <c r="A356" s="2">
@@ -8587,7 +8627,7 @@
       <c r="F356" s="2">
         <v>8.0</v>
       </c>
-      <c r="J356" s="11"/>
+      <c r="J356" s="12"/>
     </row>
     <row r="357">
       <c r="A357" s="2">
@@ -8605,7 +8645,7 @@
       <c r="F357" s="2">
         <v>14.0</v>
       </c>
-      <c r="J357" s="11"/>
+      <c r="J357" s="12"/>
     </row>
     <row r="358">
       <c r="A358" s="2">
@@ -8623,7 +8663,7 @@
       <c r="F358" s="2">
         <v>15.0</v>
       </c>
-      <c r="J358" s="11"/>
+      <c r="J358" s="12"/>
     </row>
     <row r="359">
       <c r="A359" s="9">
@@ -8704,22 +8744,22 @@
       <c r="AA360" s="4"/>
     </row>
     <row r="361">
-      <c r="A361" s="12">
+      <c r="A361" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B361" s="12" t="s">
+      <c r="B361" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C361" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D361" s="12" t="s">
+      <c r="C361" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D361" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E361" s="5"/>
       <c r="F361" s="5"/>
       <c r="G361" s="5"/>
-      <c r="H361" s="12" t="s">
+      <c r="H361" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I361" s="5"/>
@@ -8743,22 +8783,22 @@
       <c r="AA361" s="5"/>
     </row>
     <row r="362">
-      <c r="A362" s="12">
+      <c r="A362" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B362" s="12" t="s">
+      <c r="B362" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C362" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D362" s="12" t="s">
+      <c r="C362" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D362" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E362" s="5"/>
       <c r="F362" s="5"/>
       <c r="G362" s="5"/>
-      <c r="H362" s="12" t="s">
+      <c r="H362" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I362" s="5"/>
@@ -8782,22 +8822,22 @@
       <c r="AA362" s="5"/>
     </row>
     <row r="363">
-      <c r="A363" s="12">
+      <c r="A363" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B363" s="12" t="s">
+      <c r="B363" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C363" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D363" s="12" t="s">
+      <c r="C363" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D363" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E363" s="5"/>
       <c r="F363" s="5"/>
       <c r="G363" s="5"/>
-      <c r="H363" s="12" t="s">
+      <c r="H363" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I363" s="5"/>
@@ -8821,22 +8861,22 @@
       <c r="AA363" s="5"/>
     </row>
     <row r="364">
-      <c r="A364" s="12">
+      <c r="A364" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B364" s="12" t="s">
+      <c r="B364" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C364" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D364" s="12" t="s">
+      <c r="C364" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D364" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E364" s="5"/>
       <c r="F364" s="5"/>
       <c r="G364" s="5"/>
-      <c r="H364" s="12" t="s">
+      <c r="H364" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I364" s="5"/>
@@ -8860,22 +8900,22 @@
       <c r="AA364" s="5"/>
     </row>
     <row r="365">
-      <c r="A365" s="12">
+      <c r="A365" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B365" s="12" t="s">
+      <c r="B365" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C365" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D365" s="12" t="s">
+      <c r="C365" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D365" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E365" s="5"/>
       <c r="F365" s="5"/>
       <c r="G365" s="5"/>
-      <c r="H365" s="12" t="s">
+      <c r="H365" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I365" s="5"/>
@@ -8899,22 +8939,22 @@
       <c r="AA365" s="5"/>
     </row>
     <row r="366">
-      <c r="A366" s="12">
+      <c r="A366" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B366" s="12" t="s">
+      <c r="B366" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C366" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D366" s="12" t="s">
+      <c r="C366" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D366" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E366" s="5"/>
       <c r="F366" s="5"/>
       <c r="G366" s="5"/>
-      <c r="H366" s="12" t="s">
+      <c r="H366" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I366" s="5"/>
@@ -8938,22 +8978,22 @@
       <c r="AA366" s="5"/>
     </row>
     <row r="367">
-      <c r="A367" s="12">
+      <c r="A367" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B367" s="12" t="s">
+      <c r="B367" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C367" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D367" s="12" t="s">
+      <c r="C367" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D367" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E367" s="5"/>
       <c r="F367" s="5"/>
       <c r="G367" s="5"/>
-      <c r="H367" s="12" t="s">
+      <c r="H367" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I367" s="5"/>
@@ -8977,22 +9017,22 @@
       <c r="AA367" s="5"/>
     </row>
     <row r="368">
-      <c r="A368" s="12">
+      <c r="A368" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B368" s="12" t="s">
+      <c r="B368" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C368" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D368" s="12" t="s">
+      <c r="C368" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D368" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E368" s="5"/>
       <c r="F368" s="5"/>
       <c r="G368" s="5"/>
-      <c r="H368" s="12" t="s">
+      <c r="H368" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I368" s="5"/>
@@ -9016,22 +9056,22 @@
       <c r="AA368" s="5"/>
     </row>
     <row r="369">
-      <c r="A369" s="12">
+      <c r="A369" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B369" s="12" t="s">
+      <c r="B369" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C369" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D369" s="12" t="s">
+      <c r="C369" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D369" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E369" s="5"/>
       <c r="F369" s="5"/>
       <c r="G369" s="5"/>
-      <c r="H369" s="12" t="s">
+      <c r="H369" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I369" s="5"/>
@@ -9055,22 +9095,22 @@
       <c r="AA369" s="5"/>
     </row>
     <row r="370">
-      <c r="A370" s="12">
+      <c r="A370" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B370" s="12" t="s">
+      <c r="B370" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C370" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D370" s="12" t="s">
+      <c r="C370" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D370" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E370" s="5"/>
       <c r="F370" s="5"/>
       <c r="G370" s="5"/>
-      <c r="H370" s="12" t="s">
+      <c r="H370" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I370" s="5"/>
@@ -9388,7 +9428,7 @@
       <c r="F386" s="2">
         <v>9.0</v>
       </c>
-      <c r="K386" s="11"/>
+      <c r="K386" s="12"/>
     </row>
     <row r="387">
       <c r="A387" s="2">
@@ -9406,7 +9446,7 @@
       <c r="F387" s="2">
         <v>26.0</v>
       </c>
-      <c r="K387" s="11"/>
+      <c r="K387" s="12"/>
     </row>
     <row r="388">
       <c r="A388" s="2">
@@ -9424,7 +9464,7 @@
       <c r="F388" s="2">
         <v>17.0</v>
       </c>
-      <c r="K388" s="11"/>
+      <c r="K388" s="12"/>
     </row>
     <row r="389">
       <c r="A389" s="9">
@@ -9447,7 +9487,7 @@
       </c>
       <c r="I389" s="4"/>
       <c r="J389" s="4"/>
-      <c r="K389" s="13"/>
+      <c r="K389" s="14"/>
       <c r="L389" s="4"/>
       <c r="M389" s="4"/>
       <c r="N389" s="4"/>
@@ -9486,7 +9526,7 @@
       </c>
       <c r="I390" s="4"/>
       <c r="J390" s="4"/>
-      <c r="K390" s="13"/>
+      <c r="K390" s="14"/>
       <c r="L390" s="4"/>
       <c r="M390" s="4"/>
       <c r="N390" s="4"/>
@@ -9505,27 +9545,27 @@
       <c r="AA390" s="4"/>
     </row>
     <row r="391">
-      <c r="A391" s="12">
+      <c r="A391" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B391" s="12" t="s">
+      <c r="B391" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C391" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D391" s="12" t="s">
+      <c r="C391" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D391" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E391" s="5"/>
       <c r="F391" s="5"/>
       <c r="G391" s="5"/>
-      <c r="H391" s="12" t="s">
+      <c r="H391" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I391" s="5"/>
       <c r="J391" s="5"/>
-      <c r="K391" s="14"/>
+      <c r="K391" s="15"/>
       <c r="L391" s="5"/>
       <c r="M391" s="5"/>
       <c r="N391" s="5"/>
@@ -9544,27 +9584,27 @@
       <c r="AA391" s="5"/>
     </row>
     <row r="392">
-      <c r="A392" s="12">
+      <c r="A392" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B392" s="12" t="s">
+      <c r="B392" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C392" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D392" s="12" t="s">
+      <c r="C392" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D392" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E392" s="5"/>
       <c r="F392" s="5"/>
       <c r="G392" s="5"/>
-      <c r="H392" s="12" t="s">
+      <c r="H392" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I392" s="5"/>
       <c r="J392" s="5"/>
-      <c r="K392" s="14"/>
+      <c r="K392" s="15"/>
       <c r="L392" s="5"/>
       <c r="M392" s="5"/>
       <c r="N392" s="5"/>
@@ -9583,27 +9623,27 @@
       <c r="AA392" s="5"/>
     </row>
     <row r="393">
-      <c r="A393" s="12">
+      <c r="A393" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B393" s="12" t="s">
+      <c r="B393" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C393" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D393" s="12" t="s">
+      <c r="C393" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D393" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E393" s="5"/>
       <c r="F393" s="5"/>
       <c r="G393" s="5"/>
-      <c r="H393" s="12" t="s">
+      <c r="H393" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I393" s="5"/>
       <c r="J393" s="5"/>
-      <c r="K393" s="14"/>
+      <c r="K393" s="15"/>
       <c r="L393" s="5"/>
       <c r="M393" s="5"/>
       <c r="N393" s="5"/>
@@ -9622,27 +9662,27 @@
       <c r="AA393" s="5"/>
     </row>
     <row r="394">
-      <c r="A394" s="12">
+      <c r="A394" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B394" s="12" t="s">
+      <c r="B394" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C394" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D394" s="12" t="s">
+      <c r="C394" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D394" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E394" s="5"/>
       <c r="F394" s="5"/>
       <c r="G394" s="5"/>
-      <c r="H394" s="12" t="s">
+      <c r="H394" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I394" s="5"/>
       <c r="J394" s="5"/>
-      <c r="K394" s="14"/>
+      <c r="K394" s="15"/>
       <c r="L394" s="5"/>
       <c r="M394" s="5"/>
       <c r="N394" s="5"/>
@@ -9661,27 +9701,27 @@
       <c r="AA394" s="5"/>
     </row>
     <row r="395">
-      <c r="A395" s="12">
+      <c r="A395" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B395" s="12" t="s">
+      <c r="B395" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C395" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D395" s="12" t="s">
+      <c r="C395" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D395" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E395" s="5"/>
       <c r="F395" s="5"/>
       <c r="G395" s="5"/>
-      <c r="H395" s="12" t="s">
+      <c r="H395" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I395" s="5"/>
       <c r="J395" s="5"/>
-      <c r="K395" s="14"/>
+      <c r="K395" s="15"/>
       <c r="L395" s="5"/>
       <c r="M395" s="5"/>
       <c r="N395" s="5"/>
@@ -9700,27 +9740,27 @@
       <c r="AA395" s="5"/>
     </row>
     <row r="396">
-      <c r="A396" s="12">
+      <c r="A396" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B396" s="12" t="s">
+      <c r="B396" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C396" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D396" s="12" t="s">
+      <c r="C396" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D396" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E396" s="5"/>
       <c r="F396" s="5"/>
       <c r="G396" s="5"/>
-      <c r="H396" s="12" t="s">
+      <c r="H396" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I396" s="5"/>
       <c r="J396" s="5"/>
-      <c r="K396" s="14"/>
+      <c r="K396" s="15"/>
       <c r="L396" s="5"/>
       <c r="M396" s="5"/>
       <c r="N396" s="5"/>
@@ -9739,27 +9779,27 @@
       <c r="AA396" s="5"/>
     </row>
     <row r="397">
-      <c r="A397" s="12">
+      <c r="A397" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B397" s="12" t="s">
+      <c r="B397" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C397" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D397" s="12" t="s">
+      <c r="C397" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D397" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E397" s="5"/>
       <c r="F397" s="5"/>
       <c r="G397" s="5"/>
-      <c r="H397" s="12" t="s">
+      <c r="H397" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I397" s="5"/>
       <c r="J397" s="5"/>
-      <c r="K397" s="14"/>
+      <c r="K397" s="15"/>
       <c r="L397" s="5"/>
       <c r="M397" s="5"/>
       <c r="N397" s="5"/>
@@ -9778,27 +9818,27 @@
       <c r="AA397" s="5"/>
     </row>
     <row r="398">
-      <c r="A398" s="12">
+      <c r="A398" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B398" s="12" t="s">
+      <c r="B398" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C398" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D398" s="12" t="s">
+      <c r="C398" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D398" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E398" s="5"/>
       <c r="F398" s="5"/>
       <c r="G398" s="5"/>
-      <c r="H398" s="12" t="s">
+      <c r="H398" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I398" s="5"/>
       <c r="J398" s="5"/>
-      <c r="K398" s="14"/>
+      <c r="K398" s="15"/>
       <c r="L398" s="5"/>
       <c r="M398" s="5"/>
       <c r="N398" s="5"/>
@@ -9817,27 +9857,27 @@
       <c r="AA398" s="5"/>
     </row>
     <row r="399">
-      <c r="A399" s="12">
+      <c r="A399" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B399" s="12" t="s">
+      <c r="B399" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C399" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D399" s="12" t="s">
+      <c r="C399" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D399" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E399" s="5"/>
       <c r="F399" s="5"/>
       <c r="G399" s="5"/>
-      <c r="H399" s="12" t="s">
+      <c r="H399" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I399" s="5"/>
       <c r="J399" s="5"/>
-      <c r="K399" s="14"/>
+      <c r="K399" s="15"/>
       <c r="L399" s="5"/>
       <c r="M399" s="5"/>
       <c r="N399" s="5"/>
@@ -9856,22 +9896,22 @@
       <c r="AA399" s="5"/>
     </row>
     <row r="400">
-      <c r="A400" s="12">
+      <c r="A400" s="13">
         <v>2017.0</v>
       </c>
-      <c r="B400" s="12" t="s">
+      <c r="B400" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C400" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D400" s="12" t="s">
+      <c r="C400" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D400" s="13" t="s">
         <v>23</v>
       </c>
       <c r="E400" s="5"/>
       <c r="F400" s="5"/>
       <c r="G400" s="5"/>
-      <c r="H400" s="12" t="s">
+      <c r="H400" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I400" s="5"/>
@@ -9910,7 +9950,7 @@
       <c r="F401" s="2">
         <v>21.0</v>
       </c>
-      <c r="K401" s="11"/>
+      <c r="K401" s="12"/>
     </row>
     <row r="402">
       <c r="A402" s="2">
@@ -9928,7 +9968,7 @@
       <c r="F402" s="2">
         <v>29.0</v>
       </c>
-      <c r="K402" s="11"/>
+      <c r="K402" s="12"/>
     </row>
     <row r="403">
       <c r="A403" s="2">
@@ -9946,7 +9986,7 @@
       <c r="F403" s="2">
         <v>27.0</v>
       </c>
-      <c r="K403" s="11"/>
+      <c r="K403" s="12"/>
     </row>
     <row r="404">
       <c r="A404" s="2">
@@ -9964,7 +10004,7 @@
       <c r="F404" s="2">
         <v>50.0</v>
       </c>
-      <c r="K404" s="11"/>
+      <c r="K404" s="12"/>
     </row>
     <row r="405">
       <c r="A405" s="2">
@@ -9982,7 +10022,7 @@
       <c r="F405" s="2">
         <v>43.0</v>
       </c>
-      <c r="K405" s="11"/>
+      <c r="K405" s="12"/>
     </row>
     <row r="406">
       <c r="A406" s="2">
@@ -10114,22 +10154,22 @@
       <c r="AA410" s="4"/>
     </row>
     <row r="411">
-      <c r="A411" s="15">
+      <c r="A411" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B411" s="15" t="s">
+      <c r="B411" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C411" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D411" s="15" t="s">
+      <c r="C411" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D411" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E411" s="6"/>
       <c r="F411" s="6"/>
       <c r="G411" s="6"/>
-      <c r="H411" s="15" t="s">
+      <c r="H411" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I411" s="6"/>
@@ -10153,22 +10193,22 @@
       <c r="AA411" s="6"/>
     </row>
     <row r="412">
-      <c r="A412" s="15">
+      <c r="A412" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B412" s="15" t="s">
+      <c r="B412" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C412" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D412" s="15" t="s">
+      <c r="C412" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D412" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E412" s="6"/>
       <c r="F412" s="6"/>
       <c r="G412" s="6"/>
-      <c r="H412" s="15" t="s">
+      <c r="H412" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I412" s="6"/>
@@ -10192,22 +10232,22 @@
       <c r="AA412" s="6"/>
     </row>
     <row r="413">
-      <c r="A413" s="15">
+      <c r="A413" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B413" s="15" t="s">
+      <c r="B413" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C413" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D413" s="15" t="s">
+      <c r="C413" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D413" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E413" s="6"/>
       <c r="F413" s="6"/>
       <c r="G413" s="6"/>
-      <c r="H413" s="15" t="s">
+      <c r="H413" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I413" s="6"/>
@@ -10231,22 +10271,22 @@
       <c r="AA413" s="6"/>
     </row>
     <row r="414">
-      <c r="A414" s="15">
+      <c r="A414" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B414" s="15" t="s">
+      <c r="B414" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C414" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D414" s="15" t="s">
+      <c r="C414" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D414" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E414" s="6"/>
       <c r="F414" s="6"/>
       <c r="G414" s="6"/>
-      <c r="H414" s="15" t="s">
+      <c r="H414" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I414" s="6"/>
@@ -10270,22 +10310,22 @@
       <c r="AA414" s="6"/>
     </row>
     <row r="415">
-      <c r="A415" s="15">
+      <c r="A415" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B415" s="15" t="s">
+      <c r="B415" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C415" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D415" s="15" t="s">
+      <c r="C415" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D415" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E415" s="6"/>
       <c r="F415" s="6"/>
       <c r="G415" s="6"/>
-      <c r="H415" s="15" t="s">
+      <c r="H415" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I415" s="6"/>
@@ -10309,22 +10349,22 @@
       <c r="AA415" s="6"/>
     </row>
     <row r="416">
-      <c r="A416" s="15">
+      <c r="A416" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B416" s="15" t="s">
+      <c r="B416" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C416" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D416" s="15" t="s">
+      <c r="C416" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D416" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E416" s="6"/>
       <c r="F416" s="6"/>
       <c r="G416" s="6"/>
-      <c r="H416" s="15" t="s">
+      <c r="H416" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I416" s="6"/>
@@ -10348,22 +10388,22 @@
       <c r="AA416" s="6"/>
     </row>
     <row r="417">
-      <c r="A417" s="15">
+      <c r="A417" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B417" s="15" t="s">
+      <c r="B417" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C417" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D417" s="15" t="s">
+      <c r="C417" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D417" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E417" s="6"/>
       <c r="F417" s="6"/>
       <c r="G417" s="6"/>
-      <c r="H417" s="15" t="s">
+      <c r="H417" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I417" s="6"/>
@@ -10387,22 +10427,22 @@
       <c r="AA417" s="6"/>
     </row>
     <row r="418">
-      <c r="A418" s="15">
+      <c r="A418" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B418" s="15" t="s">
+      <c r="B418" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C418" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D418" s="15" t="s">
+      <c r="C418" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D418" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E418" s="6"/>
       <c r="F418" s="6"/>
       <c r="G418" s="6"/>
-      <c r="H418" s="15" t="s">
+      <c r="H418" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I418" s="6"/>
@@ -10426,22 +10466,22 @@
       <c r="AA418" s="6"/>
     </row>
     <row r="419">
-      <c r="A419" s="15">
+      <c r="A419" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B419" s="15" t="s">
+      <c r="B419" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C419" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D419" s="15" t="s">
+      <c r="C419" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D419" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E419" s="6"/>
       <c r="F419" s="6"/>
       <c r="G419" s="6"/>
-      <c r="H419" s="15" t="s">
+      <c r="H419" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I419" s="6"/>
@@ -10465,22 +10505,22 @@
       <c r="AA419" s="6"/>
     </row>
     <row r="420">
-      <c r="A420" s="15">
+      <c r="A420" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B420" s="15" t="s">
+      <c r="B420" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C420" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D420" s="15" t="s">
+      <c r="C420" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D420" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E420" s="6"/>
       <c r="F420" s="6"/>
       <c r="G420" s="6"/>
-      <c r="H420" s="15" t="s">
+      <c r="H420" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I420" s="6"/>
@@ -10607,7 +10647,7 @@
       <c r="F427" s="2">
         <v>7.0</v>
       </c>
-      <c r="K427" s="11"/>
+      <c r="K427" s="12"/>
     </row>
     <row r="428">
       <c r="A428" s="2">
@@ -10623,7 +10663,7 @@
       <c r="F428" s="2">
         <v>8.0</v>
       </c>
-      <c r="K428" s="11"/>
+      <c r="K428" s="12"/>
     </row>
     <row r="429">
       <c r="A429" s="9">
@@ -10644,7 +10684,7 @@
       </c>
       <c r="I429" s="4"/>
       <c r="J429" s="4"/>
-      <c r="K429" s="13"/>
+      <c r="K429" s="14"/>
       <c r="L429" s="4"/>
       <c r="M429" s="4"/>
       <c r="N429" s="4"/>
@@ -10732,7 +10772,7 @@
       <c r="F432" s="16">
         <v>28.0</v>
       </c>
-      <c r="K432" s="11"/>
+      <c r="K432" s="12"/>
     </row>
     <row r="433">
       <c r="A433" s="2">
@@ -10750,7 +10790,7 @@
       <c r="F433" s="16">
         <v>20.0</v>
       </c>
-      <c r="K433" s="11"/>
+      <c r="K433" s="12"/>
     </row>
     <row r="434">
       <c r="A434" s="2">
@@ -10785,7 +10825,7 @@
       <c r="F435" s="16">
         <v>49.0</v>
       </c>
-      <c r="K435" s="11"/>
+      <c r="K435" s="12"/>
     </row>
     <row r="436">
       <c r="A436" s="2">
@@ -10917,22 +10957,22 @@
       <c r="AA440" s="4"/>
     </row>
     <row r="441">
-      <c r="A441" s="15">
+      <c r="A441" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B441" s="15" t="s">
+      <c r="B441" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C441" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D441" s="15" t="s">
+      <c r="C441" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D441" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E441" s="6"/>
       <c r="F441" s="6"/>
       <c r="G441" s="6"/>
-      <c r="H441" s="15" t="s">
+      <c r="H441" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I441" s="6"/>
@@ -10956,22 +10996,22 @@
       <c r="AA441" s="6"/>
     </row>
     <row r="442">
-      <c r="A442" s="15">
+      <c r="A442" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B442" s="15" t="s">
+      <c r="B442" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C442" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D442" s="15" t="s">
+      <c r="C442" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D442" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E442" s="6"/>
       <c r="F442" s="6"/>
       <c r="G442" s="6"/>
-      <c r="H442" s="15" t="s">
+      <c r="H442" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I442" s="6"/>
@@ -10995,22 +11035,22 @@
       <c r="AA442" s="6"/>
     </row>
     <row r="443">
-      <c r="A443" s="15">
+      <c r="A443" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B443" s="15" t="s">
+      <c r="B443" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C443" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D443" s="15" t="s">
+      <c r="C443" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D443" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E443" s="6"/>
       <c r="F443" s="6"/>
       <c r="G443" s="6"/>
-      <c r="H443" s="15" t="s">
+      <c r="H443" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I443" s="6"/>
@@ -11034,22 +11074,22 @@
       <c r="AA443" s="6"/>
     </row>
     <row r="444">
-      <c r="A444" s="15">
+      <c r="A444" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B444" s="15" t="s">
+      <c r="B444" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C444" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D444" s="15" t="s">
+      <c r="C444" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D444" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E444" s="6"/>
       <c r="F444" s="6"/>
       <c r="G444" s="6"/>
-      <c r="H444" s="15" t="s">
+      <c r="H444" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I444" s="6"/>
@@ -11073,22 +11113,22 @@
       <c r="AA444" s="6"/>
     </row>
     <row r="445">
-      <c r="A445" s="15">
+      <c r="A445" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B445" s="15" t="s">
+      <c r="B445" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C445" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D445" s="15" t="s">
+      <c r="C445" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D445" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E445" s="6"/>
       <c r="F445" s="6"/>
       <c r="G445" s="6"/>
-      <c r="H445" s="15" t="s">
+      <c r="H445" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I445" s="6"/>
@@ -11112,22 +11152,22 @@
       <c r="AA445" s="6"/>
     </row>
     <row r="446">
-      <c r="A446" s="15">
+      <c r="A446" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B446" s="15" t="s">
+      <c r="B446" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C446" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D446" s="15" t="s">
+      <c r="C446" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D446" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E446" s="6"/>
       <c r="F446" s="6"/>
       <c r="G446" s="6"/>
-      <c r="H446" s="15" t="s">
+      <c r="H446" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I446" s="6"/>
@@ -11151,22 +11191,22 @@
       <c r="AA446" s="6"/>
     </row>
     <row r="447">
-      <c r="A447" s="15">
+      <c r="A447" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B447" s="15" t="s">
+      <c r="B447" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C447" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D447" s="15" t="s">
+      <c r="C447" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D447" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E447" s="6"/>
       <c r="F447" s="6"/>
       <c r="G447" s="6"/>
-      <c r="H447" s="15" t="s">
+      <c r="H447" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I447" s="6"/>
@@ -11190,22 +11230,22 @@
       <c r="AA447" s="6"/>
     </row>
     <row r="448">
-      <c r="A448" s="15">
+      <c r="A448" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B448" s="15" t="s">
+      <c r="B448" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C448" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D448" s="15" t="s">
+      <c r="C448" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D448" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E448" s="6"/>
       <c r="F448" s="6"/>
       <c r="G448" s="6"/>
-      <c r="H448" s="15" t="s">
+      <c r="H448" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I448" s="6"/>
@@ -11229,22 +11269,22 @@
       <c r="AA448" s="6"/>
     </row>
     <row r="449">
-      <c r="A449" s="15">
+      <c r="A449" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B449" s="15" t="s">
+      <c r="B449" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C449" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D449" s="15" t="s">
+      <c r="C449" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D449" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E449" s="6"/>
       <c r="F449" s="6"/>
       <c r="G449" s="6"/>
-      <c r="H449" s="15" t="s">
+      <c r="H449" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I449" s="6"/>
@@ -11268,22 +11308,22 @@
       <c r="AA449" s="6"/>
     </row>
     <row r="450">
-      <c r="A450" s="15">
+      <c r="A450" s="10">
         <v>2016.0</v>
       </c>
-      <c r="B450" s="15" t="s">
+      <c r="B450" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C450" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D450" s="15" t="s">
+      <c r="C450" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D450" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E450" s="6"/>
       <c r="F450" s="6"/>
       <c r="G450" s="6"/>
-      <c r="H450" s="15" t="s">
+      <c r="H450" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I450" s="6"/>
@@ -11521,22 +11561,22 @@
       <c r="AA460" s="4"/>
     </row>
     <row r="461">
-      <c r="A461" s="15">
+      <c r="A461" s="10">
         <v>2015.0</v>
       </c>
-      <c r="B461" s="15" t="s">
+      <c r="B461" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C461" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D461" s="15" t="s">
+      <c r="C461" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D461" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E461" s="6"/>
       <c r="F461" s="6"/>
       <c r="G461" s="6"/>
-      <c r="H461" s="15" t="s">
+      <c r="H461" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I461" s="6"/>
@@ -11560,22 +11600,22 @@
       <c r="AA461" s="6"/>
     </row>
     <row r="462">
-      <c r="A462" s="15">
+      <c r="A462" s="10">
         <v>2015.0</v>
       </c>
-      <c r="B462" s="15" t="s">
+      <c r="B462" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C462" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D462" s="15" t="s">
+      <c r="C462" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D462" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E462" s="6"/>
       <c r="F462" s="6"/>
       <c r="G462" s="6"/>
-      <c r="H462" s="15" t="s">
+      <c r="H462" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I462" s="6"/>
@@ -11599,22 +11639,22 @@
       <c r="AA462" s="6"/>
     </row>
     <row r="463">
-      <c r="A463" s="15">
+      <c r="A463" s="10">
         <v>2015.0</v>
       </c>
-      <c r="B463" s="15" t="s">
+      <c r="B463" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C463" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D463" s="15" t="s">
+      <c r="C463" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D463" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E463" s="6"/>
       <c r="F463" s="6"/>
       <c r="G463" s="6"/>
-      <c r="H463" s="15" t="s">
+      <c r="H463" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I463" s="6"/>
@@ -11638,22 +11678,22 @@
       <c r="AA463" s="6"/>
     </row>
     <row r="464">
-      <c r="A464" s="15">
+      <c r="A464" s="10">
         <v>2015.0</v>
       </c>
-      <c r="B464" s="15" t="s">
+      <c r="B464" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C464" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D464" s="15" t="s">
+      <c r="C464" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D464" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E464" s="6"/>
       <c r="F464" s="6"/>
       <c r="G464" s="6"/>
-      <c r="H464" s="15" t="s">
+      <c r="H464" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I464" s="6"/>
@@ -11677,22 +11717,22 @@
       <c r="AA464" s="6"/>
     </row>
     <row r="465">
-      <c r="A465" s="15">
+      <c r="A465" s="10">
         <v>2015.0</v>
       </c>
-      <c r="B465" s="15" t="s">
+      <c r="B465" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C465" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D465" s="15" t="s">
+      <c r="C465" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D465" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E465" s="6"/>
       <c r="F465" s="6"/>
       <c r="G465" s="6"/>
-      <c r="H465" s="15" t="s">
+      <c r="H465" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I465" s="6"/>
@@ -11716,22 +11756,22 @@
       <c r="AA465" s="6"/>
     </row>
     <row r="466">
-      <c r="A466" s="15">
+      <c r="A466" s="10">
         <v>2015.0</v>
       </c>
-      <c r="B466" s="15" t="s">
+      <c r="B466" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C466" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D466" s="15" t="s">
+      <c r="C466" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D466" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E466" s="6"/>
       <c r="F466" s="6"/>
       <c r="G466" s="6"/>
-      <c r="H466" s="15" t="s">
+      <c r="H466" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I466" s="6"/>
@@ -11755,22 +11795,22 @@
       <c r="AA466" s="6"/>
     </row>
     <row r="467">
-      <c r="A467" s="15">
+      <c r="A467" s="10">
         <v>2015.0</v>
       </c>
-      <c r="B467" s="15" t="s">
+      <c r="B467" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C467" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D467" s="15" t="s">
+      <c r="C467" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D467" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E467" s="6"/>
       <c r="F467" s="6"/>
       <c r="G467" s="6"/>
-      <c r="H467" s="15" t="s">
+      <c r="H467" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I467" s="6"/>
@@ -11794,22 +11834,22 @@
       <c r="AA467" s="6"/>
     </row>
     <row r="468">
-      <c r="A468" s="15">
+      <c r="A468" s="10">
         <v>2015.0</v>
       </c>
-      <c r="B468" s="15" t="s">
+      <c r="B468" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C468" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D468" s="15" t="s">
+      <c r="C468" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D468" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E468" s="6"/>
       <c r="F468" s="6"/>
       <c r="G468" s="6"/>
-      <c r="H468" s="15" t="s">
+      <c r="H468" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I468" s="6"/>
@@ -11833,22 +11873,22 @@
       <c r="AA468" s="6"/>
     </row>
     <row r="469">
-      <c r="A469" s="15">
+      <c r="A469" s="10">
         <v>2015.0</v>
       </c>
-      <c r="B469" s="15" t="s">
+      <c r="B469" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C469" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D469" s="15" t="s">
+      <c r="C469" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D469" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E469" s="6"/>
       <c r="F469" s="6"/>
       <c r="G469" s="6"/>
-      <c r="H469" s="15" t="s">
+      <c r="H469" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I469" s="6"/>
@@ -11872,22 +11912,22 @@
       <c r="AA469" s="6"/>
     </row>
     <row r="470">
-      <c r="A470" s="15">
+      <c r="A470" s="10">
         <v>2015.0</v>
       </c>
-      <c r="B470" s="15" t="s">
+      <c r="B470" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C470" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D470" s="15" t="s">
+      <c r="C470" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D470" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E470" s="6"/>
       <c r="F470" s="6"/>
       <c r="G470" s="6"/>
-      <c r="H470" s="15" t="s">
+      <c r="H470" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I470" s="6"/>

</xml_diff>